<commit_message>
Penambahan Rekayasa Perangkat Lunak
</commit_message>
<xml_diff>
--- a/kerangka berpikir.xlsx
+++ b/kerangka berpikir.xlsx
@@ -85,9 +85,6 @@
     <t>Sistem harus bisa mencatat aktivitas keuangan dan memproses menjadi laporan buku besar.</t>
   </si>
   <si>
-    <t>Harus ada aplikasi yang bisa membantu pencatatan aktivitas keuangan untuk meminimalkan kesalahan pencatatan dan menambah efisiensi waktu.</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Banyaknya kesalahan pada pengelompokan debit dan kredit. </t>
+  </si>
+  <si>
+    <t>Dihasilkan aplikasi yang bisa membantu pencatatan aktivitas keuangan untuk meminimalkan kesalahan pencatatan dan menambah efisiensi waktu.</t>
   </si>
 </sst>
 </file>
@@ -234,22 +234,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -788,17 +788,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -814,34 +814,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
     </row>
     <row r="6" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="10"/>
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -850,42 +850,42 @@
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:2" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>10</v>
@@ -894,17 +894,17 @@
     <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>